<commit_message>
added documentation, made correction to code generating scalar morphometrics table
</commit_message>
<xml_diff>
--- a/GJMorph/etc/DL-Int-1_globalMeasuresSpec.xlsx
+++ b/GJMorph/etc/DL-Int-1_globalMeasuresSpec.xlsx
@@ -73,7 +73,7 @@
     <t xml:space="preserve">Total dendritic length</t>
   </si>
   <si>
-    <t xml:space="preserve">(x10^4 \mu m)</t>
+    <t xml:space="preserve">x10^4 \mu m</t>
   </si>
   <si>
     <t xml:space="preserve">Total Length</t>
@@ -82,7 +82,7 @@
     <t xml:space="preserve">Total dendritic surface</t>
   </si>
   <si>
-    <t xml:space="preserve">(x10^4 \mu m^2)</t>
+    <t xml:space="preserve">x10^4 \mu m^2</t>
   </si>
   <si>
     <t xml:space="preserve">Total Surface</t>
@@ -91,7 +91,7 @@
     <t xml:space="preserve">Total dendritic Volume</t>
   </si>
   <si>
-    <t xml:space="preserve">(x10^4 \mu m^3)</t>
+    <t xml:space="preserve">x10^4 \mu m^3</t>
   </si>
   <si>
     <t xml:space="preserve">Total Volume</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Avg. bifurcation angle (local)</t>
   </si>
   <si>
-    <t xml:space="preserve">'(\text{degrees})'</t>
+    <t xml:space="preserve">\text{degrees}</t>
   </si>
   <si>
     <t xml:space="preserve">avg_bif_angle_local</t>
@@ -278,14 +278,14 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="31.8112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="9.96428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="32.030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.0714285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.6428571428571"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="1" width="8.78571428571429"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.1377551020408"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="1" width="11.780612244898"/>

</xml_diff>